<commit_message>
Some small changes in views
</commit_message>
<xml_diff>
--- a/API-documentation-usedbikes.xlsx
+++ b/API-documentation-usedbikes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajayb\OneDrive\Desktop\Luminar Projects\olx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86CB82D-3332-4191-A2DB-3CEA46E438C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AB6979-6691-4B66-ADD2-873051283D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -253,13 +253,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -545,7 +545,7 @@
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27:O27"/>
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -554,173 +554,173 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
       <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13" t="s">
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13" t="s">
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="13"/>
+      <c r="Q1" s="9"/>
       <c r="R1" s="6"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
       <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9" t="s">
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q3" s="9"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="10"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
       <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9" t="s">
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q4" s="9"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="10"/>
     </row>
     <row r="5" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
       <c r="G6" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9" t="s">
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q6" s="9"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q6" s="10"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
       <c r="G7" t="s">
         <v>15</v>
       </c>
@@ -743,14 +743,14 @@
       <c r="R7" s="7"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
       <c r="G8" t="s">
         <v>15</v>
       </c>
@@ -773,14 +773,14 @@
       <c r="R8" s="3"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
       <c r="G9" t="s">
         <v>20</v>
       </c>
@@ -803,14 +803,14 @@
       <c r="R9" s="3"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
       <c r="G10" t="s">
         <v>22</v>
       </c>
@@ -833,14 +833,14 @@
       <c r="R10" s="3"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
       <c r="G11" t="s">
         <v>7</v>
       </c>
@@ -863,14 +863,14 @@
       <c r="R11" s="3"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
       <c r="G12" t="s">
         <v>15</v>
       </c>
@@ -893,14 +893,14 @@
       <c r="R12" s="3"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
       <c r="G13" t="s">
         <v>7</v>
       </c>
@@ -923,14 +923,14 @@
       <c r="R13" s="3"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
       <c r="G14" t="s">
         <v>15</v>
       </c>
@@ -953,14 +953,14 @@
       <c r="R14" s="3"/>
     </row>
     <row r="15" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="4" t="s">
         <v>7</v>
       </c>
@@ -983,35 +983,35 @@
       <c r="R15" s="5"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
       <c r="G17" t="s">
         <v>15</v>
       </c>
@@ -1034,14 +1034,14 @@
       <c r="R17" s="3"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
       <c r="G18" t="s">
         <v>15</v>
       </c>
@@ -1064,14 +1064,14 @@
       <c r="R18" s="3"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
       <c r="G19" t="s">
         <v>39</v>
       </c>
@@ -1094,14 +1094,14 @@
       <c r="R19" s="3"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
       <c r="G20" t="s">
         <v>22</v>
       </c>
@@ -1124,35 +1124,35 @@
       <c r="R20" s="3"/>
     </row>
     <row r="21" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
       <c r="G22" t="s">
         <v>15</v>
       </c>
@@ -1175,14 +1175,14 @@
       <c r="R22" s="3"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
       <c r="G23" t="s">
         <v>7</v>
       </c>
@@ -1205,14 +1205,14 @@
       <c r="R23" s="3"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
       <c r="G24" t="s">
         <v>7</v>
       </c>
@@ -1234,35 +1234,35 @@
       <c r="Q24" s="8"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
       <c r="G26" t="s">
         <v>15</v>
       </c>
@@ -1284,14 +1284,14 @@
       <c r="Q26" s="8"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
       <c r="G27" t="s">
         <v>15</v>
       </c>
@@ -1313,57 +1313,65 @@
       <c r="Q27" s="8"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="97">
-    <mergeCell ref="H26:L26"/>
-    <mergeCell ref="A25:Q25"/>
-    <mergeCell ref="M28:O28"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="H22:L22"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="H15:L15"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="H14:L14"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="A16:Q16"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="A21:Q21"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="H27:L27"/>
+    <mergeCell ref="H28:L28"/>
+    <mergeCell ref="H23:L23"/>
+    <mergeCell ref="H24:L24"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="A5:Q5"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="A2:Q2"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
     <mergeCell ref="M4:O4"/>
     <mergeCell ref="M6:O6"/>
     <mergeCell ref="A27:F27"/>
@@ -1380,55 +1388,47 @@
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="A24:F24"/>
     <mergeCell ref="A14:F14"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="A16:Q16"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="M17:O17"/>
     <mergeCell ref="A17:F17"/>
     <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="H15:L15"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="A25:Q25"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="H22:L22"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="H20:L20"/>
     <mergeCell ref="H19:L19"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="A2:Q2"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="A5:Q5"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="A8:F8"/>
     <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="A21:Q21"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="H27:L27"/>
-    <mergeCell ref="H28:L28"/>
-    <mergeCell ref="H23:L23"/>
-    <mergeCell ref="H24:L24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>